<commit_message>
ajout au DF de données geographiques et politiques (ancien ministre/membre du gouvernement)
</commit_message>
<xml_diff>
--- a/legislatives/data/geographie_depart.xlsx
+++ b/legislatives/data/geographie_depart.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projet_fil_rouge\Elections\legislatives\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>dep</t>
   </si>
@@ -22,12 +27,6 @@
     <t>depart_frontalier</t>
   </si>
   <si>
-    <t>depart_OM</t>
-  </si>
-  <si>
-    <t>depart_CORSE</t>
-  </si>
-  <si>
     <t>region_parisienne</t>
   </si>
   <si>
@@ -350,13 +349,16 @@
   </si>
   <si>
     <t>HAUTE-CORSE</t>
+  </si>
+  <si>
+    <t>depart_DOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,11 +421,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -465,7 +475,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,9 +507,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,6 +559,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -706,14 +752,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,22 +775,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -746,16 +797,13 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -766,16 +814,13 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -786,16 +831,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -806,16 +848,13 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -826,16 +865,13 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -846,16 +882,13 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>319</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -866,16 +899,13 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>358</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -886,16 +916,13 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>387</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -906,16 +933,13 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>409</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -926,16 +950,13 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>446</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -946,16 +967,13 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>490</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -966,16 +984,13 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>518</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -986,16 +1001,13 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>783</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1006,16 +1018,13 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>868</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1026,16 +1035,13 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>890</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1046,16 +1052,13 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>929</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1066,16 +1069,13 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1003</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1086,16 +1086,13 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1034</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1106,16 +1103,13 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1060</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1126,16 +1120,13 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1128</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1146,16 +1137,13 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1191</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1166,16 +1154,13 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1205</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1186,16 +1171,13 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1252</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1206,16 +1188,13 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1305</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1226,16 +1205,13 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1366</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1246,16 +1222,13 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1432</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1266,16 +1239,13 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1484</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1286,16 +1256,13 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1596</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1306,16 +1273,13 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1680</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1326,16 +1290,13 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1821</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1346,16 +1307,13 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1848</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1366,16 +1324,13 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2025</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1386,16 +1341,13 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2157</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1406,16 +1358,13 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2272</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1426,16 +1375,13 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2297</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1446,16 +1392,13 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2364</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1466,16 +1409,13 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2486</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1486,16 +1426,13 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2520</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1506,16 +1443,13 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2557</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1526,16 +1460,13 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2589</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1546,16 +1477,13 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2660</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1566,16 +1494,13 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2683</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1586,16 +1511,13 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2839</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1606,16 +1528,13 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2916</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1626,16 +1545,13 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2937</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1646,16 +1562,13 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2975</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1666,16 +1579,13 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2988</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1686,16 +1596,13 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>3072</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1706,16 +1613,13 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>3117</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1726,16 +1630,13 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>3175</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1746,16 +1647,13 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>3195</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1766,16 +1664,13 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>3232</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1786,16 +1681,13 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>3314</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1806,16 +1698,13 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>3336</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1826,16 +1715,13 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>3416</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1846,16 +1732,13 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>3552</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1866,16 +1749,13 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>3580</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1886,16 +1766,13 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>3861</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1906,16 +1783,13 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>3945</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1926,16 +1800,13 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>3979</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1946,16 +1817,13 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>4124</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1966,16 +1834,13 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>4185</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1986,16 +1851,13 @@
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>4266</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2006,16 +1868,13 @@
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>4292</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2026,16 +1885,13 @@
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>4344</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2046,16 +1902,13 @@
       <c r="E67">
         <v>0</v>
       </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>4476</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2066,16 +1919,13 @@
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>4567</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2086,16 +1936,13 @@
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>4783</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2106,16 +1953,13 @@
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>4809</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2126,16 +1970,13 @@
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>4875</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2146,16 +1987,13 @@
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>4941</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2166,16 +2004,13 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>4994</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2186,16 +2021,13 @@
       <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>5077</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2204,18 +2036,15 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>5451</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2226,16 +2055,13 @@
       <c r="E76">
         <v>0</v>
       </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>5568</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2244,18 +2070,15 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>5700</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2264,18 +2087,15 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>5875</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2286,16 +2106,13 @@
       <c r="E79">
         <v>0</v>
       </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>5905</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2306,16 +2123,13 @@
       <c r="E80">
         <v>0</v>
       </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>5957</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2326,16 +2140,13 @@
       <c r="E81">
         <v>0</v>
       </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>5998</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2346,16 +2157,13 @@
       <c r="E82">
         <v>0</v>
       </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>6023</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2366,16 +2174,13 @@
       <c r="E83">
         <v>0</v>
       </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>6142</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2386,16 +2191,13 @@
       <c r="E84">
         <v>0</v>
       </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>6211</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2406,16 +2208,13 @@
       <c r="E85">
         <v>0</v>
       </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>6271</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2426,16 +2225,13 @@
       <c r="E86">
         <v>0</v>
       </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>6322</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2446,16 +2242,13 @@
       <c r="E87">
         <v>0</v>
       </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>6357</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2466,16 +2259,13 @@
       <c r="E88">
         <v>0</v>
       </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>6406</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2486,16 +2276,13 @@
       <c r="E89">
         <v>0</v>
       </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>6449</v>
       </c>
       <c r="B90" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2506,16 +2293,13 @@
       <c r="E90">
         <v>0</v>
       </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>6472</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2524,18 +2308,15 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>6616</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2544,18 +2325,15 @@
         <v>0</v>
       </c>
       <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>6829</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2564,18 +2342,15 @@
         <v>0</v>
       </c>
       <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>7007</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2584,18 +2359,15 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>7160</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2604,18 +2376,15 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>0</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>7314</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -2626,16 +2395,13 @@
       <c r="E96">
         <v>0</v>
       </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>7496</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -2646,16 +2412,13 @@
       <c r="E97">
         <v>0</v>
       </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>7578</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -2666,16 +2429,13 @@
       <c r="E98">
         <v>0</v>
       </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>7631</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -2686,76 +2446,64 @@
       <c r="E99">
         <v>0</v>
       </c>
-      <c r="F99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>7650</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>7739</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>7744</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>7757</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -2766,107 +2514,89 @@
       <c r="E103">
         <v>0</v>
       </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>7789</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C104">
         <v>0</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
-      <c r="F104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>7792</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C105">
         <v>0</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>7819</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C106">
         <v>0</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
-      <c r="F106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>7841</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107">
-        <v>1</v>
-      </c>
-      <c r="F107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>7859</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108">
         <v>0</v>
       </c>
     </row>

</xml_diff>